<commit_message>
MON-551 add nested joins
</commit_message>
<xml_diff>
--- a/tests/Feature/JoinTest/joinable_dummies.xlsx
+++ b/tests/Feature/JoinTest/joinable_dummies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">another_joinable_relations.another_foreign_field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another_joinable_relations.nested_joinable_relations.foreign_field</t>
   </si>
   <si>
     <t xml:space="preserve">title 1</t>
@@ -196,10 +199,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -232,27 +235,33 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -261,21 +270,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -284,21 +296,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>